<commit_message>
Automatische test-sync: 2025-08-19 19:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,8 +725,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:17:12</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -746,7 +788,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -754,17 +796,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -806,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,8 +767,50 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:29:14</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -788,7 +830,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -796,17 +838,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -848,7 +890,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,8 +809,50 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:33:57</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -830,7 +872,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -838,17 +880,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -890,7 +932,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,8 +851,50 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Demo inplannen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:39:13</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -872,7 +914,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -880,17 +922,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -932,7 +974,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,8 +893,50 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:41:24</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -914,7 +956,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -922,17 +964,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -974,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,8 +935,50 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:43:33</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -956,7 +998,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -964,17 +1006,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1016,7 +1058,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -977,8 +977,50 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CE-certificaten verzoek</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>inkoop@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:45:42</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -998,7 +1040,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1006,17 +1048,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1058,7 +1100,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1019,8 +1019,50 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>support@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:47:54</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1040,7 +1082,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1048,17 +1090,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1100,7 +1142,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:50:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,8 +1061,50 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>klantenservice@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:50:03</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1082,7 +1124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1090,17 +1132,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1184,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,8 +1103,50 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Datasheet opvragen</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>retour@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:52:14</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1124,7 +1166,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1132,17 +1174,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1184,7 +1226,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,8 +1145,50 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:54:27</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1166,7 +1208,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1174,17 +1216,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1226,7 +1268,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,8 +1187,50 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:56:38</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1208,7 +1250,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1216,17 +1258,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1268,7 +1310,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 19:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1229,8 +1229,50 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Algemene vraag</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>klachten@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-19 19:58:52</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1250,7 +1292,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1258,17 +1300,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1310,7 +1352,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 20:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1271,8 +1271,50 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-19 20:24:05</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1292,7 +1334,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1300,17 +1342,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1352,7 +1394,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 20:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,8 +1313,50 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-19 20:25:36</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1334,7 +1376,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1342,17 +1384,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1394,7 +1436,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 20:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1355,8 +1355,50 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-19 20:44:25</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1376,7 +1418,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1384,17 +1426,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1436,7 +1478,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 20:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1397,8 +1397,50 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>planning@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-19 20:54:06</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1418,7 +1460,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1426,17 +1468,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1478,7 +1520,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 20:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,8 +1439,50 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-19 20:59:11</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1460,7 +1502,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1468,17 +1510,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1520,7 +1562,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 21:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,8 +1481,50 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-19 21:01:05</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1502,7 +1544,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1510,17 +1552,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1562,7 +1604,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 21:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,8 +1523,50 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-19 21:02:55</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1544,7 +1586,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1552,17 +1594,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1604,7 +1646,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 21:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1565,8 +1565,50 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-19 21:04:22</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1586,7 +1628,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1594,17 +1636,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1646,7 +1688,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 21:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1607,8 +1607,50 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Vraag over product</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>documentatie@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-19 21:07:36</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1628,7 +1670,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1636,17 +1678,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1688,7 +1730,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-19 21:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-19.xlsx
+++ b/logs/mail_log_2025-08-19.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1649,8 +1649,50 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-19 21:10:46</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1670,7 +1712,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1678,17 +1720,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1730,7 +1772,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>